<commit_message>
TEst Cases + Purcahser Inteview Logic
Finshied test caes for purchaser
Started building in hlepful labels in inteview structure
</commit_message>
<xml_diff>
--- a/GST_AT_SETTLEMENT/Tests/Purchaser.xlsx
+++ b/GST_AT_SETTLEMENT/Tests/Purchaser.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Documents\GitHub\IT_Law_Assignment\GST_AT_SETTLEMENT\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{07D613F5-C118-452D-B9B6-FE83FD410476}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5DEDE7EA-04F3-48BD-B12D-CD4CFE69B046}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3285" yWindow="105" windowWidth="19320" windowHeight="12120" tabRatio="255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>Test Case</t>
   </si>
@@ -70,13 +70,43 @@
     <t>Base Case - True</t>
   </si>
   <si>
-    <t>Base Case - One Exception</t>
-  </si>
-  <si>
     <t>Branch -Transitional Rules - Exception</t>
   </si>
   <si>
     <t>Branch -Transitional Rules - Pass</t>
+  </si>
+  <si>
+    <t>the property is of 'potential residential land'</t>
+  </si>
+  <si>
+    <t>the property is included in a 'property subdivision plan'</t>
+  </si>
+  <si>
+    <t>the property contains any building that is in use for a commercial purpose</t>
+  </si>
+  <si>
+    <t>the purchaser is registered for GST</t>
+  </si>
+  <si>
+    <t>the supply has been created through substantial renovations</t>
+  </si>
+  <si>
+    <t>Base Case - One Exception *unknown</t>
+  </si>
+  <si>
+    <t>the supply is of commercial residential premises</t>
+  </si>
+  <si>
+    <t>the purchaser is registered but does not purchase the property for a creditable purpose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branch - Resdiential Premise Or Potential Rediential Land - Residential Land One Attribute </t>
+  </si>
+  <si>
+    <t>Branch - Resdiential Premise Or Potential Rediential Land - Residential Premise -Full Logic</t>
+  </si>
+  <si>
+    <t>Branch - Resdiential Premise Or Potential Rediential Land - Residential Premise -Full Logic - End Exception</t>
   </si>
 </sst>
 </file>
@@ -749,11 +779,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD6"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -765,15 +795,22 @@
     <col min="5" max="5" width="42.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="53.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.85546875" customWidth="1"/>
-    <col min="12" max="12" width="34" style="10" customWidth="1"/>
-    <col min="13" max="13" width="42.85546875" customWidth="1"/>
+    <col min="8" max="8" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" customWidth="1"/>
+    <col min="11" max="11" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="33.85546875" customWidth="1"/>
+    <col min="19" max="19" width="34" style="10" customWidth="1"/>
+    <col min="20" max="20" width="68.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -796,26 +833,47 @@
         <v>3</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="4" t="s">
+      <c r="M1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="S1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="T1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="2"/>
+      <c r="V1" s="2"/>
     </row>
-    <row r="2" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -831,26 +889,33 @@
       <c r="G2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="L2" s="11" t="s">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="R2" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="S2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="T2" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -866,26 +931,33 @@
       <c r="G3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" s="14" t="s">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="R3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="S3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="12" t="s">
-        <v>16</v>
+      <c r="T3" s="12" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -907,26 +979,33 @@
       <c r="G4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H4" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K4" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="L4" s="11" t="s">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="R4" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="S4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="12" t="s">
-        <v>18</v>
+      <c r="T4" s="12" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -948,36 +1027,204 @@
       <c r="G5" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H5" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K5" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="11" t="s">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R5" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="S5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="12" t="s">
-        <v>17</v>
+      <c r="T5" s="12" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+    <row r="6" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="R6" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="S6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="T6" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="R7" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="S7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="T7" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="R8" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="S8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="T8" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>